<commit_message>
Resolved errors with merged file.
</commit_message>
<xml_diff>
--- a/data/CFUViol_merge.xlsx
+++ b/data/CFUViol_merge.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-20" windowWidth="12800" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,8 +129,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -165,7 +169,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -179,6 +183,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -192,6 +198,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -720,6 +728,9 @@
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -742,9 +753,12 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3">
-        <v>42172</v>
+        <v>42171</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="1"/>
@@ -770,10 +784,13 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3">
-        <v>42173</v>
+        <v>42171</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
@@ -815,11 +832,11 @@
         <v>3</v>
       </c>
       <c r="G8" s="2">
-        <f>(20*(1/D8))*E8</f>
+        <f t="shared" ref="G8:G25" si="2">(20*(1/D8))*E8</f>
         <v>11000000000</v>
       </c>
       <c r="H8" s="2">
-        <f>(20*(1/D8))*F8</f>
+        <f t="shared" ref="H8:H25" si="3">(20*(1/D8))*F8</f>
         <v>600000000</v>
       </c>
       <c r="I8" s="2">
@@ -861,11 +878,11 @@
         <v>13</v>
       </c>
       <c r="G9" s="2">
-        <f>(20*(1/D9))*E9</f>
+        <f t="shared" si="2"/>
         <v>7200000000</v>
       </c>
       <c r="H9" s="2">
-        <f>(20*(1/D9))*F9</f>
+        <f t="shared" si="3"/>
         <v>2600000000</v>
       </c>
       <c r="I9" s="2">
@@ -907,11 +924,11 @@
         <v>4</v>
       </c>
       <c r="G10" s="2">
-        <f>(20*(1/D10))*E10</f>
+        <f t="shared" si="2"/>
         <v>10600000000</v>
       </c>
       <c r="H10" s="2">
-        <f>(20*(1/D10))*F10</f>
+        <f t="shared" si="3"/>
         <v>800000000</v>
       </c>
       <c r="I10" s="2">
@@ -953,11 +970,11 @@
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <f>(20*(1/D11))*E11</f>
+        <f t="shared" si="2"/>
         <v>8600000000</v>
       </c>
       <c r="H11" s="2">
-        <f>(20*(1/D11))*F11</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I11" s="2">
@@ -999,11 +1016,11 @@
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <f>(20*(1/D12))*E12</f>
+        <f t="shared" si="2"/>
         <v>11400000000</v>
       </c>
       <c r="H12" s="2">
-        <f>(20*(1/D12))*F12</f>
+        <f t="shared" si="3"/>
         <v>200000000</v>
       </c>
       <c r="I12" s="2">
@@ -1045,11 +1062,11 @@
         <v>1</v>
       </c>
       <c r="G13" s="2">
-        <f>(20*(1/D13))*E13</f>
+        <f t="shared" si="2"/>
         <v>10200000000</v>
       </c>
       <c r="H13" s="2">
-        <f>(20*(1/D13))*F13</f>
+        <f t="shared" si="3"/>
         <v>200000000</v>
       </c>
       <c r="I13" s="2">
@@ -1091,11 +1108,11 @@
         <v>49</v>
       </c>
       <c r="G14" s="2">
-        <f>(20*(1/D14))*E14</f>
+        <f t="shared" si="2"/>
         <v>8100000000</v>
       </c>
       <c r="H14" s="2">
-        <f>(20*(1/D14))*F14</f>
+        <f t="shared" si="3"/>
         <v>980000000</v>
       </c>
       <c r="I14" s="2">
@@ -1136,11 +1153,11 @@
         <v>27</v>
       </c>
       <c r="G15" s="2">
-        <f>(20*(1/D15))*E15</f>
+        <f t="shared" si="2"/>
         <v>3500000000</v>
       </c>
       <c r="H15" s="2">
-        <f>(20*(1/D15))*F15</f>
+        <f t="shared" si="3"/>
         <v>540000000</v>
       </c>
       <c r="I15" s="2">
@@ -1181,11 +1198,11 @@
         <v>41</v>
       </c>
       <c r="G16" s="2">
-        <f>(20*(1/D16))*E16</f>
+        <f t="shared" si="2"/>
         <v>3460000000</v>
       </c>
       <c r="H16" s="2">
-        <f>(20*(1/D16))*F16</f>
+        <f t="shared" si="3"/>
         <v>820000000</v>
       </c>
       <c r="I16" s="2">
@@ -1226,11 +1243,11 @@
         <v>179</v>
       </c>
       <c r="G17" s="2">
-        <f>(20*(1/D17))*E17</f>
+        <f t="shared" si="2"/>
         <v>4480000000</v>
       </c>
       <c r="H17" s="2">
-        <f>(20*(1/D17))*F17</f>
+        <f t="shared" si="3"/>
         <v>3580000000</v>
       </c>
       <c r="I17" s="2">
@@ -1271,11 +1288,11 @@
         <v>25</v>
       </c>
       <c r="G18" s="2">
-        <f>(20*(1/D18))*E18</f>
+        <f t="shared" si="2"/>
         <v>6680000000</v>
       </c>
       <c r="H18" s="2">
-        <f>(20*(1/D18))*F18</f>
+        <f t="shared" si="3"/>
         <v>500000000</v>
       </c>
       <c r="I18" s="2">
@@ -1316,11 +1333,11 @@
         <v>47</v>
       </c>
       <c r="G19" s="2">
-        <f>(20*(1/D19))*E19</f>
+        <f t="shared" si="2"/>
         <v>6860000000</v>
       </c>
       <c r="H19" s="2">
-        <f>(20*(1/D19))*F19</f>
+        <f t="shared" si="3"/>
         <v>940000000</v>
       </c>
       <c r="I19" s="2">
@@ -1361,11 +1378,11 @@
         <v>35</v>
       </c>
       <c r="G20" s="2">
-        <f>(20*(1/D20))*E20</f>
+        <f t="shared" si="2"/>
         <v>5240000000</v>
       </c>
       <c r="H20" s="2">
-        <f>(20*(1/D20))*F20</f>
+        <f t="shared" si="3"/>
         <v>700000000</v>
       </c>
       <c r="I20" s="2">
@@ -1407,11 +1424,11 @@
         <v>208</v>
       </c>
       <c r="G21" s="2">
-        <f>(20*(1/D21))*E21</f>
+        <f t="shared" si="2"/>
         <v>4120000000</v>
       </c>
       <c r="H21" s="2">
-        <f>(20*(1/D21))*F21</f>
+        <f t="shared" si="3"/>
         <v>4160000000</v>
       </c>
       <c r="I21" s="2">
@@ -1452,11 +1469,11 @@
         <v>84</v>
       </c>
       <c r="G22" s="2">
-        <f>(20*(1/D22))*E22</f>
+        <f t="shared" si="2"/>
         <v>4700000000</v>
       </c>
       <c r="H22" s="2">
-        <f>(20*(1/D22))*F22</f>
+        <f t="shared" si="3"/>
         <v>1680000000</v>
       </c>
       <c r="I22" s="2">
@@ -1498,11 +1515,11 @@
         <v>62</v>
       </c>
       <c r="G23" s="2">
-        <f>(20*(1/D23))*E23</f>
+        <f t="shared" si="2"/>
         <v>4100000000</v>
       </c>
       <c r="H23" s="2">
-        <f>(20*(1/D23))*F23</f>
+        <f t="shared" si="3"/>
         <v>1240000000</v>
       </c>
       <c r="I23" s="2">
@@ -1544,11 +1561,11 @@
         <v>84</v>
       </c>
       <c r="G24" s="2">
-        <f>(20*(1/D24))*E24</f>
+        <f t="shared" si="2"/>
         <v>4360000000</v>
       </c>
       <c r="H24" s="2">
-        <f>(20*(1/D24))*F24</f>
+        <f t="shared" si="3"/>
         <v>1680000000</v>
       </c>
       <c r="I24" s="2">
@@ -1590,11 +1607,11 @@
         <v>24</v>
       </c>
       <c r="G25" s="2">
-        <f>(20*(1/D25))*E25</f>
+        <f t="shared" si="2"/>
         <v>5560000000</v>
       </c>
       <c r="H25" s="2">
-        <f>(20*(1/D25))*F25</f>
+        <f t="shared" si="3"/>
         <v>480000000</v>
       </c>
       <c r="I25" s="2">
@@ -1832,15 +1849,15 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" ref="G33:G55" si="2">(20*(1/D33))*E33</f>
+        <f t="shared" ref="G33:G55" si="4">(20*(1/D33))*E33</f>
         <v>185999999.99999997</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" ref="H33:H55" si="3">(20*(1/D33))*F33</f>
+        <f t="shared" ref="H33:H55" si="5">(20*(1/D33))*F33</f>
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" ref="I33:I55" si="4">G33/(G33+H33)</f>
+        <f t="shared" ref="I33:I55" si="6">G33/(G33+H33)</f>
         <v>1</v>
       </c>
       <c r="J33" s="2">
@@ -1854,13 +1871,13 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33:M61" si="5">((K33-L33)/J33)*1000</f>
+        <f t="shared" ref="M33:M61" si="7">((K33-L33)/J33)*1000</f>
         <v>2.4742268041237123</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="3">
-        <v>42171</v>
+        <v>42170</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>3</v>
@@ -1885,7 +1902,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2121212121212133</v>
       </c>
     </row>
@@ -1909,15 +1926,15 @@
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11999999.999999998</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J35" s="2">
@@ -1930,13 +1947,13 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.3188262446422694</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="3">
-        <v>42171</v>
+        <v>42170</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>1</v>
@@ -1961,13 +1978,13 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.97276264591439765</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="3">
-        <v>42172</v>
+        <v>42170</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
@@ -1991,7 +2008,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.6561775422325287</v>
       </c>
     </row>
@@ -2015,15 +2032,15 @@
         <v>1</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21999999.999999996</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1999999.9999999998</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="J38" s="2">
@@ -2037,7 +2054,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.5472088215024122</v>
       </c>
     </row>
@@ -2061,15 +2078,15 @@
         <v>0</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27999999.999999996</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J39" s="2">
@@ -2083,7 +2100,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.5153395380903136</v>
       </c>
     </row>
@@ -2107,15 +2124,15 @@
         <v>0</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33999999.999999993</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J40" s="2">
@@ -2129,7 +2146,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.460674157303373</v>
       </c>
     </row>
@@ -2153,15 +2170,15 @@
         <v>0</v>
       </c>
       <c r="G41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23999999.999999996</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J41" s="2">
@@ -2175,7 +2192,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11.702127659574467</v>
       </c>
     </row>
@@ -2199,15 +2216,15 @@
         <v>2</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>53999999.999999993</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3999999.9999999995</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.93103448275862066</v>
       </c>
       <c r="J42" s="2">
@@ -2220,7 +2237,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15.075376884422109</v>
       </c>
     </row>
@@ -2244,15 +2261,15 @@
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39999999.999999993</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J43" s="2">
@@ -2266,7 +2283,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15.591397849462364</v>
       </c>
     </row>
@@ -2290,15 +2307,15 @@
         <v>13</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25999999.999999996</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J44" s="2">
@@ -2312,7 +2329,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>41.812865497076025</v>
       </c>
     </row>
@@ -2336,15 +2353,15 @@
         <v>16</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>31999999.999999996</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J45" s="2">
@@ -2358,7 +2375,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7989821882951662</v>
       </c>
     </row>
@@ -2382,15 +2399,15 @@
         <v>12</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23999999.999999996</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J46" s="2">
@@ -2403,7 +2420,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.6548672566371687</v>
       </c>
     </row>
@@ -2427,15 +2444,15 @@
         <v>12</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23999999.999999996</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J47" s="2">
@@ -2448,7 +2465,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.5959595959595969</v>
       </c>
     </row>
@@ -2472,15 +2489,15 @@
         <v>16</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>31999999.999999996</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J48" s="2">
@@ -2493,7 +2510,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>109.11680911680912</v>
       </c>
     </row>
@@ -2517,15 +2534,15 @@
         <v>70</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15999999.999999998</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>139999999.99999997</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.10256410256410257</v>
       </c>
       <c r="J49" s="2">
@@ -2538,7 +2555,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>25.543478260869566</v>
       </c>
     </row>
@@ -2562,15 +2579,15 @@
         <v>96</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>200000</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19200000</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0309278350515464E-2</v>
       </c>
       <c r="J50" s="2">
@@ -2583,7 +2600,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>17.283950617283953</v>
       </c>
     </row>
@@ -2607,15 +2624,15 @@
         <v>210</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42000000</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J51" s="2">
@@ -2628,7 +2645,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16.695059625212949</v>
       </c>
     </row>
@@ -2652,15 +2669,15 @@
         <v>116</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23200000</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J52" s="2">
@@ -2673,7 +2690,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>43.080054274084119</v>
       </c>
     </row>
@@ -2697,15 +2714,15 @@
         <v>150</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>30000000</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J53" s="2">
@@ -2718,7 +2735,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>30.060120240480963</v>
       </c>
     </row>
@@ -2742,15 +2759,15 @@
         <v>57</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>200000</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11400000</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.7241379310344827E-2</v>
       </c>
       <c r="J54" s="2">
@@ -2763,7 +2780,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44.731610337972164</v>
       </c>
     </row>
@@ -2787,15 +2804,15 @@
         <v>137</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>27400000</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J55" s="2">
@@ -2809,7 +2826,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.1240105540897094</v>
       </c>
     </row>
@@ -2833,7 +2850,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.0286360211002261</v>
       </c>
     </row>
@@ -2857,7 +2874,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.9904458598726107</v>
       </c>
     </row>
@@ -2881,7 +2898,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.9607843137254892</v>
       </c>
     </row>
@@ -2905,7 +2922,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.2632342277012332</v>
       </c>
     </row>
@@ -2929,7 +2946,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6072144288577159</v>
       </c>
     </row>
@@ -2953,7 +2970,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.409443269908385</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data files with latest colony count information.
</commit_message>
<xml_diff>
--- a/data/CFUViol_merge.xlsx
+++ b/data/CFUViol_merge.xlsx
@@ -129,8 +129,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,7 +173,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -185,6 +189,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -200,6 +206,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -531,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I25" si="0">G3/(G3+H3)</f>
+        <f t="shared" ref="I3:I31" si="0">G3/(G3+H3)</f>
         <v>1</v>
       </c>
       <c r="J3" s="2">
@@ -832,11 +840,11 @@
         <v>3</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" ref="G8:G25" si="2">(20*(1/D8))*E8</f>
+        <f t="shared" ref="G8:G31" si="2">(20*(1/D8))*E8</f>
         <v>11000000000</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ref="H8:H25" si="3">(20*(1/D8))*F8</f>
+        <f t="shared" ref="H8:H31" si="3">(20*(1/D8))*F8</f>
         <v>600000000</v>
       </c>
       <c r="I8" s="2">
@@ -1643,6 +1651,27 @@
       <c r="C26">
         <v>1</v>
       </c>
+      <c r="D26" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E26" s="2">
+        <v>317</v>
+      </c>
+      <c r="F26" s="2">
+        <v>124</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>6340000000</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="3"/>
+        <v>2480000000</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.71882086167800452</v>
+      </c>
       <c r="J26" s="2">
         <f>0.495*10</f>
         <v>4.95</v>
@@ -1668,6 +1697,27 @@
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="D27" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E27" s="2">
+        <v>245</v>
+      </c>
+      <c r="F27" s="2">
+        <v>111</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>4900000000</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="3"/>
+        <v>2220000000</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6882022471910112</v>
+      </c>
       <c r="J27" s="2">
         <f>0.531*10</f>
         <v>5.3100000000000005</v>
@@ -1693,6 +1743,27 @@
       <c r="C28">
         <v>1</v>
       </c>
+      <c r="D28" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E28" s="2">
+        <v>302</v>
+      </c>
+      <c r="F28" s="2">
+        <v>141</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>6040000000</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="3"/>
+        <v>2820000000</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.68171557562076746</v>
+      </c>
       <c r="J28" s="2">
         <f>0.51*10</f>
         <v>5.0999999999999996</v>
@@ -1718,6 +1789,27 @@
       <c r="C29">
         <v>1</v>
       </c>
+      <c r="D29" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E29" s="2">
+        <v>178</v>
+      </c>
+      <c r="F29" s="2">
+        <v>150</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>3560000000</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="3"/>
+        <v>3000000000</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54268292682926833</v>
+      </c>
       <c r="J29" s="2">
         <f>0.507*10</f>
         <v>5.07</v>
@@ -1743,6 +1835,27 @@
       <c r="C30">
         <v>1</v>
       </c>
+      <c r="D30" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>231</v>
+      </c>
+      <c r="F30" s="2">
+        <v>103</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>4620000000</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="3"/>
+        <v>2060000000</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.69161676646706582</v>
+      </c>
       <c r="J30" s="2">
         <f>0.524*10</f>
         <v>5.24</v>
@@ -1768,6 +1881,27 @@
       <c r="C31">
         <v>1</v>
       </c>
+      <c r="D31" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E31" s="2">
+        <v>324</v>
+      </c>
+      <c r="F31" s="2">
+        <v>21</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>6480000000</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="3"/>
+        <v>420000000</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.93913043478260871</v>
+      </c>
       <c r="J31" s="2">
         <f>0.505*10</f>
         <v>5.05</v>
@@ -1849,15 +1983,15 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" ref="G33:G55" si="4">(20*(1/D33))*E33</f>
+        <f t="shared" ref="G33:G56" si="4">(20*(1/D33))*E33</f>
         <v>185999999.99999997</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" ref="H33:H55" si="5">(20*(1/D33))*F33</f>
+        <f t="shared" ref="H33:H61" si="5">(20*(1/D33))*F33</f>
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" ref="I33:I55" si="6">G33/(G33+H33)</f>
+        <f t="shared" ref="I33:I56" si="6">G33/(G33+H33)</f>
         <v>1</v>
       </c>
       <c r="J33" s="2">
@@ -2840,6 +2974,27 @@
       <c r="C56">
         <v>10</v>
       </c>
+      <c r="D56" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2">
+        <v>262</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="5"/>
+        <v>52400000</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="J56" s="2">
         <v>2.6539999999999999</v>
       </c>
@@ -2864,6 +3019,19 @@
       <c r="C57">
         <v>10</v>
       </c>
+      <c r="D57" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>64</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="5"/>
+        <v>12800000</v>
+      </c>
       <c r="J57" s="2">
         <v>2.512</v>
       </c>
@@ -2888,6 +3056,19 @@
       <c r="C58">
         <v>10</v>
       </c>
+      <c r="D58" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>189</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="5"/>
+        <v>37800000</v>
+      </c>
       <c r="J58" s="2">
         <v>2.5499999999999998</v>
       </c>
@@ -2912,6 +3093,19 @@
       <c r="C59">
         <v>10</v>
       </c>
+      <c r="D59" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>14</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="5"/>
+        <v>2800000</v>
+      </c>
       <c r="J59" s="2">
         <v>2.758</v>
       </c>
@@ -2936,6 +3130,19 @@
       <c r="C60">
         <v>10</v>
       </c>
+      <c r="D60" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2">
+        <v>17</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="5"/>
+        <v>3400000</v>
+      </c>
       <c r="J60" s="2">
         <v>2.4950000000000001</v>
       </c>
@@ -2959,6 +3166,19 @@
       </c>
       <c r="C61">
         <v>10</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2">
+        <v>162</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="5"/>
+        <v>32400000</v>
       </c>
       <c r="J61" s="2">
         <v>2.8380000000000001</v>

</xml_diff>

<commit_message>
Additional data file addtions.
</commit_message>
<xml_diff>
--- a/data/CFUViol_merge.xlsx
+++ b/data/CFUViol_merge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="5700" yWindow="0" windowWidth="24640" windowHeight="12640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,8 +129,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -173,7 +183,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -191,6 +201,11 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -208,6 +223,11 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,7 +560,7 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:E61"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1983,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" ref="G33:G56" si="4">(20*(1/D33))*E33</f>
+        <f t="shared" ref="G33:G61" si="4">(20*(1/D33))*E33</f>
         <v>185999999.99999997</v>
       </c>
       <c r="H33" s="2">
@@ -1991,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" ref="I33:I56" si="6">G33/(G33+H33)</f>
+        <f t="shared" ref="I33:I61" si="6">G33/(G33+H33)</f>
         <v>1</v>
       </c>
       <c r="J33" s="2">
@@ -3028,10 +3048,18 @@
       <c r="F57" s="2">
         <v>64</v>
       </c>
+      <c r="G57" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="H57" s="2">
         <f t="shared" si="5"/>
         <v>12800000</v>
       </c>
+      <c r="I57" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="J57" s="2">
         <v>2.512</v>
       </c>
@@ -3065,10 +3093,18 @@
       <c r="F58" s="2">
         <v>189</v>
       </c>
+      <c r="G58" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="H58" s="2">
         <f t="shared" si="5"/>
         <v>37800000</v>
       </c>
+      <c r="I58" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="J58" s="2">
         <v>2.5499999999999998</v>
       </c>
@@ -3102,10 +3138,18 @@
       <c r="F59" s="2">
         <v>14</v>
       </c>
+      <c r="G59" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="H59" s="2">
         <f t="shared" si="5"/>
         <v>2800000</v>
       </c>
+      <c r="I59" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="J59" s="2">
         <v>2.758</v>
       </c>
@@ -3139,10 +3183,18 @@
       <c r="F60" s="2">
         <v>17</v>
       </c>
+      <c r="G60" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="H60" s="2">
         <f t="shared" si="5"/>
         <v>3400000</v>
       </c>
+      <c r="I60" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="J60" s="2">
         <v>2.4950000000000001</v>
       </c>
@@ -3176,9 +3228,17 @@
       <c r="F61" s="2">
         <v>162</v>
       </c>
+      <c r="G61" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="H61" s="2">
         <f t="shared" si="5"/>
         <v>32400000</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="J61" s="2">
         <v>2.8380000000000001</v>

</xml_diff>